<commit_message>
Committing the Login Application File.
</commit_message>
<xml_diff>
--- a/LoginApplication/Resources/JavaReadValues.xlsx
+++ b/LoginApplication/Resources/JavaReadValues.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginInformation" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CustomerName</t>
   </si>
@@ -36,10 +36,22 @@
     <t>Chev</t>
   </si>
   <si>
-    <t>chebatch</t>
-  </si>
-  <si>
-    <t>Batchrun22</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>TradBatch</t>
+  </si>
+  <si>
+    <t>http://gb2trpec-001.ffastserve.com/j2ee/</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -403,16 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -443,6 +455,20 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>